<commit_message>
Added tables and generally cleaned things up
</commit_message>
<xml_diff>
--- a/Final hand written solutions.xlsx
+++ b/Final hand written solutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lando\Desktop\Fall 2020\Financial Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0956E94-8DBC-4BAF-99C2-E683DF86EF64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3031EF8-AE0A-44F7-9632-BDD7C58C33DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part1- problem 1b" sheetId="4" r:id="rId1"/>
@@ -148,8 +148,8 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -613,12 +613,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -630,11 +630,11 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -645,7 +645,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -668,24 +668,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,6 +700,24 @@
     <xf numFmtId="44" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1151,7 +1151,7 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1200,15 +1200,15 @@
         <f>EXP(($C$6-$C$8)*$C$11+$C$7*SQRT($C$11))</f>
         <v>1.3231298123374369</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="47"/>
+      <c r="J3" s="64"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="50"/>
+      <c r="M3" s="66"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
       <c r="A4" s="2"/>
@@ -1248,10 +1248,10 @@
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="53"/>
+      <c r="J5" s="47"/>
       <c r="K5" s="21"/>
       <c r="L5" s="23"/>
-      <c r="M5" s="53"/>
+      <c r="M5" s="47"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="2"/>
@@ -1271,10 +1271,10 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="27"/>
-      <c r="J6" s="54"/>
+      <c r="J6" s="48"/>
       <c r="K6" s="21"/>
       <c r="L6" s="27"/>
-      <c r="M6" s="54"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="2"/>
@@ -1287,13 +1287,13 @@
       <c r="D7" s="2"/>
       <c r="H7" s="14"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="55">
+      <c r="J7" s="49">
         <f>$F$3*I8</f>
         <v>132.3129812337437</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="27"/>
-      <c r="M7" s="55">
+      <c r="M7" s="49">
         <f>MAX(J7-$C$4,0)</f>
         <v>27.312981233743699</v>
       </c>
@@ -1311,13 +1311,13 @@
         <f>$C$3</f>
         <v>100</v>
       </c>
-      <c r="J8" s="56"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="21"/>
       <c r="L8" s="31">
         <f>$F$6*($F$5*$M$7+(1-$F$5)*$M$9)</f>
         <v>11.350062186067705</v>
       </c>
-      <c r="M8" s="56"/>
+      <c r="M8" s="50"/>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2"/>
@@ -1325,13 +1325,13 @@
       <c r="D9" s="2"/>
       <c r="H9" s="14"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="55">
+      <c r="J9" s="49">
         <f>$F$4*I8</f>
         <v>88.692043671715751</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="27"/>
-      <c r="M9" s="55">
+      <c r="M9" s="49">
         <f>MAX(J9-$C$4,0)</f>
         <v>0</v>
       </c>
@@ -1347,10 +1347,10 @@
       <c r="D10" s="2"/>
       <c r="H10" s="14"/>
       <c r="I10" s="27"/>
-      <c r="J10" s="54"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="21"/>
       <c r="L10" s="27"/>
-      <c r="M10" s="54"/>
+      <c r="M10" s="48"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="2"/>
@@ -1364,30 +1364,30 @@
       <c r="D11" s="2"/>
       <c r="H11" s="14"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="57"/>
+      <c r="J11" s="51"/>
       <c r="K11" s="21"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="51"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1">
       <c r="A12" s="2"/>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="2"/>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="58">
-        <v>0</v>
-      </c>
-      <c r="J12" s="59">
+      <c r="I12" s="52">
+        <v>0</v>
+      </c>
+      <c r="J12" s="53">
         <v>1</v>
       </c>
-      <c r="K12" s="52"/>
-      <c r="L12" s="68">
-        <v>0</v>
-      </c>
-      <c r="M12" s="65">
+      <c r="K12" s="46"/>
+      <c r="L12" s="62">
+        <v>0</v>
+      </c>
+      <c r="M12" s="59">
         <v>1</v>
       </c>
     </row>
@@ -1396,15 +1396,15 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="47"/>
+      <c r="J14" s="64"/>
       <c r="K14" s="21"/>
-      <c r="L14" s="48" t="s">
+      <c r="L14" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="50"/>
+      <c r="M14" s="66"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15" s="2"/>
@@ -1418,30 +1418,30 @@
       <c r="A16" s="2"/>
       <c r="H16" s="14"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="53"/>
+      <c r="J16" s="47"/>
       <c r="K16" s="21"/>
       <c r="L16" s="23"/>
-      <c r="M16" s="53"/>
+      <c r="M16" s="47"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2"/>
       <c r="H17" s="14"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="54"/>
+      <c r="J17" s="48"/>
       <c r="K17" s="21"/>
       <c r="L17" s="27"/>
-      <c r="M17" s="54"/>
+      <c r="M17" s="48"/>
     </row>
     <row r="18" spans="1:13">
       <c r="H18" s="14"/>
       <c r="I18" s="27"/>
-      <c r="J18" s="55">
+      <c r="J18" s="49">
         <f>$F$3*I19</f>
         <v>132.3129812337437</v>
       </c>
       <c r="K18" s="21"/>
       <c r="L18" s="27"/>
-      <c r="M18" s="55">
+      <c r="M18" s="49">
         <f>MAX($C$4-J18,0)</f>
         <v>0</v>
       </c>
@@ -1452,25 +1452,25 @@
         <f>$C$3</f>
         <v>100</v>
       </c>
-      <c r="J19" s="56"/>
+      <c r="J19" s="50"/>
       <c r="K19" s="21"/>
       <c r="L19" s="31">
         <f>$F$6*($F$5*M18+(1-$F$5)*M20)</f>
         <v>8.2772785566644487</v>
       </c>
-      <c r="M19" s="56"/>
+      <c r="M19" s="50"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2"/>
       <c r="H20" s="14"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="55">
+      <c r="J20" s="49">
         <f>$F$4*I19</f>
         <v>88.692043671715751</v>
       </c>
       <c r="K20" s="21"/>
       <c r="L20" s="27"/>
-      <c r="M20" s="55">
+      <c r="M20" s="49">
         <f>MAX($C$4-J20,0)</f>
         <v>16.307956328284249</v>
       </c>
@@ -1479,18 +1479,18 @@
       <c r="A21" s="2"/>
       <c r="H21" s="14"/>
       <c r="I21" s="27"/>
-      <c r="J21" s="54"/>
+      <c r="J21" s="48"/>
       <c r="K21" s="21"/>
       <c r="L21" s="27"/>
-      <c r="M21" s="54"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="1:13" ht="15" thickBot="1">
       <c r="H22" s="14"/>
       <c r="I22" s="34"/>
-      <c r="J22" s="57"/>
+      <c r="J22" s="51"/>
       <c r="K22" s="21"/>
       <c r="L22" s="34"/>
-      <c r="M22" s="57"/>
+      <c r="M22" s="51"/>
     </row>
     <row r="23" spans="1:13" ht="16.5" thickBot="1">
       <c r="A23" s="3"/>
@@ -1498,20 +1498,20 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="H23" s="51" t="s">
+      <c r="H23" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="58">
-        <v>0</v>
-      </c>
-      <c r="J23" s="59">
+      <c r="I23" s="52">
+        <v>0</v>
+      </c>
+      <c r="J23" s="53">
         <v>1</v>
       </c>
-      <c r="K23" s="52"/>
-      <c r="L23" s="68">
-        <v>0</v>
-      </c>
-      <c r="M23" s="65">
+      <c r="K23" s="46"/>
+      <c r="L23" s="62">
+        <v>0</v>
+      </c>
+      <c r="M23" s="59">
         <v>1</v>
       </c>
     </row>
@@ -1590,19 +1590,19 @@
         <f>EXP(($C$6-$C$8)*$C$11+$C$7*SQRT($C$11))</f>
         <v>1.1527342401707321</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="21"/>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="50"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="66"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1">
       <c r="A4" s="2"/>
@@ -1648,7 +1648,7 @@
       <c r="I5" s="23"/>
       <c r="J5" s="24"/>
       <c r="K5" s="25"/>
-      <c r="L5" s="66">
+      <c r="L5" s="60">
         <f>$F$3*K6</f>
         <v>153.17489107578726</v>
       </c>
@@ -1692,7 +1692,7 @@
         <f>$F$6*($F$5*Q5+(1-$F$5)*Q7)</f>
         <v>30.642619164119282</v>
       </c>
-      <c r="Q6" s="61"/>
+      <c r="Q6" s="55"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2"/>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="P7" s="17"/>
       <c r="Q7" s="30">
-        <f t="shared" ref="Q7:Q11" si="0">MAX(L7-$C$4,0)</f>
+        <f t="shared" ref="Q7" si="0">MAX(L7-$C$4,0)</f>
         <v>16.588238236609442</v>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="L8" s="29"/>
       <c r="M8" s="21"/>
-      <c r="N8" s="62">
+      <c r="N8" s="56">
         <f>$F$6*($F$5*O7+(1-$F$5)*O9)</f>
         <v>10.044685209190392</v>
       </c>
@@ -1755,7 +1755,7 @@
         <f>$F$6*($F$5*Q7+(1-$F$5)*Q9)</f>
         <v>7.6101226489536993</v>
       </c>
-      <c r="Q8" s="61"/>
+      <c r="Q8" s="55"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="P9" s="17"/>
       <c r="Q9" s="30">
-        <f t="shared" ref="Q9:Q12" si="1">MAX(L9-$C$4,0)</f>
+        <f t="shared" ref="Q9" si="1">MAX(L9-$C$4,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1808,7 +1808,7 @@
         <f>$F$6*($F$5*Q9+(1-$F$5)*Q11)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="61"/>
+      <c r="Q10" s="55"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1">
       <c r="A11" s="2"/>
@@ -1833,7 +1833,7 @@
       <c r="O11" s="35"/>
       <c r="P11" s="36"/>
       <c r="Q11" s="37">
-        <f t="shared" ref="Q11:Q12" si="2">MAX(L11-$C$4,0)</f>
+        <f t="shared" ref="Q11" si="2">MAX(L11-$C$4,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1858,16 +1858,16 @@
         <v>3</v>
       </c>
       <c r="M12" s="22"/>
-      <c r="N12" s="68">
-        <v>0</v>
-      </c>
-      <c r="O12" s="64">
+      <c r="N12" s="62">
+        <v>0</v>
+      </c>
+      <c r="O12" s="58">
         <v>1</v>
       </c>
-      <c r="P12" s="64">
+      <c r="P12" s="58">
         <v>2</v>
       </c>
-      <c r="Q12" s="65">
+      <c r="Q12" s="59">
         <v>3</v>
       </c>
     </row>
@@ -1876,19 +1876,19 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="47"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="64"/>
       <c r="M14" s="21"/>
-      <c r="N14" s="48" t="s">
+      <c r="N14" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="50"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="66"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1">
       <c r="A15" s="2"/>
@@ -1938,7 +1938,7 @@
         <f>$F$6*($F$5*$Q$16+(1-$F$5)*$Q$18)</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="61"/>
+      <c r="Q17" s="55"/>
     </row>
     <row r="18" spans="1:17">
       <c r="H18" s="14"/>
@@ -1986,7 +1986,7 @@
         <f>$F$6*($F$5*$Q$18+(1-$F$5)*$Q$20)</f>
         <v>4.3690083056676121</v>
       </c>
-      <c r="Q19" s="61"/>
+      <c r="Q19" s="55"/>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="2"/>
@@ -2030,7 +2030,7 @@
         <f>$F$6*($F$5*$Q$20+(1-$F$5)*$Q$22)</f>
         <v>18.509844138209566</v>
       </c>
-      <c r="Q21" s="61"/>
+      <c r="Q21" s="55"/>
     </row>
     <row r="22" spans="1:17" ht="15" thickBot="1">
       <c r="H22" s="14"/>
@@ -2067,16 +2067,16 @@
         <v>3</v>
       </c>
       <c r="M23" s="22"/>
-      <c r="N23" s="68">
-        <v>0</v>
-      </c>
-      <c r="O23" s="64">
+      <c r="N23" s="62">
+        <v>0</v>
+      </c>
+      <c r="O23" s="58">
         <v>1</v>
       </c>
-      <c r="P23" s="64">
+      <c r="P23" s="58">
         <v>2</v>
       </c>
-      <c r="Q23" s="65">
+      <c r="Q23" s="59">
         <v>3</v>
       </c>
     </row>
@@ -2099,8 +2099,8 @@
   </sheetPr>
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -2153,19 +2153,19 @@
         <f>EXP(($C$6-$C$8)*$C$11+$C$7*SQRT($C$11))</f>
         <v>1.2212461201543867</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="47"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="21"/>
-      <c r="O3" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="50"/>
+      <c r="O3" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="66"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1">
       <c r="A4" s="2"/>
@@ -2211,8 +2211,8 @@
       <c r="J5" s="23"/>
       <c r="K5" s="24"/>
       <c r="L5" s="25"/>
-      <c r="M5" s="26">
-        <f>L6*F3</f>
+      <c r="M5" s="18">
+        <f>$F$3*L6</f>
         <v>182.14178609528693</v>
       </c>
       <c r="N5" s="21"/>
@@ -2243,8 +2243,8 @@
       <c r="I6" s="14"/>
       <c r="J6" s="27"/>
       <c r="K6" s="28"/>
-      <c r="L6" s="19">
-        <f>F3*K7</f>
+      <c r="L6" s="18">
+        <f>$F$3*K7</f>
         <v>149.14420859921427</v>
       </c>
       <c r="M6" s="29"/>
@@ -2255,7 +2255,7 @@
         <f>MAX($F$6*($F$5*R5+(1-$F$5)*R7),L6-$C$4)</f>
         <v>56.644062410665491</v>
       </c>
-      <c r="R6" s="61"/>
+      <c r="R6" s="55"/>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="2"/>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="30">
-        <f>L6*F4</f>
+        <f>L6*$F$4</f>
         <v>128.81474239966511</v>
       </c>
       <c r="N7" s="21"/>
@@ -2299,17 +2299,17 @@
       </c>
       <c r="D8" s="2"/>
       <c r="J8" s="31">
-        <f>C3</f>
+        <f>$C$3</f>
         <v>100</v>
       </c>
       <c r="K8" s="16"/>
-      <c r="L8" s="19">
-        <f>K7*F4</f>
+      <c r="L8" s="30">
+        <f>K7*$F$4</f>
         <v>105.47811802536633</v>
       </c>
       <c r="M8" s="29"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="62">
+      <c r="O8" s="56">
         <f>MAX($F$6*($F$5*P7+(1-$F$5)*P9),J8-$C$4)</f>
         <v>18.282552207370557</v>
       </c>
@@ -2318,7 +2318,7 @@
         <f>MAX($F$6*($F$5*R7+(1-$F$5)*R9),L8-$C$4)</f>
         <v>15.040328553689362</v>
       </c>
-      <c r="R8" s="61"/>
+      <c r="R8" s="55"/>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="2"/>
@@ -2326,13 +2326,13 @@
       <c r="D9" s="2"/>
       <c r="I9" s="14"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="18">
-        <f>$F$4*J8</f>
+      <c r="K9" s="30">
+        <f>J8*$F$4</f>
         <v>86.369255373382117</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="30">
-        <f>L8*F4</f>
+        <f>L8*$F$4</f>
         <v>91.100665120366031</v>
       </c>
       <c r="N9" s="21"/>
@@ -2359,8 +2359,8 @@
       <c r="I10" s="14"/>
       <c r="J10" s="27"/>
       <c r="K10" s="28"/>
-      <c r="L10" s="19">
-        <f>K9*F4</f>
+      <c r="L10" s="30">
+        <f>K9*$F$4</f>
         <v>74.596482737524951</v>
       </c>
       <c r="M10" s="29"/>
@@ -2371,7 +2371,7 @@
         <f>MAX($F$6*($F$5*R9+(1-$F$5)*R11),L10-$C$4)</f>
         <v>0</v>
       </c>
-      <c r="R10" s="61"/>
+      <c r="R10" s="55"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1">
       <c r="A11" s="2"/>
@@ -2387,8 +2387,8 @@
       <c r="J11" s="34"/>
       <c r="K11" s="35"/>
       <c r="L11" s="36"/>
-      <c r="M11" s="37">
-        <f>L10*F4</f>
+      <c r="M11" s="30">
+        <f>L10*$F$4</f>
         <v>64.428426675133835</v>
       </c>
       <c r="N11" s="21"/>
@@ -2405,32 +2405,32 @@
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
       <c r="D12" s="2"/>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="58">
-        <v>0</v>
-      </c>
-      <c r="K12" s="63">
+      <c r="J12" s="52">
+        <v>0</v>
+      </c>
+      <c r="K12" s="57">
         <v>1</v>
       </c>
-      <c r="L12" s="64">
+      <c r="L12" s="58">
         <v>2</v>
       </c>
-      <c r="M12" s="65">
+      <c r="M12" s="59">
         <v>3</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="68">
-        <v>0</v>
-      </c>
-      <c r="P12" s="64">
+      <c r="N12" s="46"/>
+      <c r="O12" s="62">
+        <v>0</v>
+      </c>
+      <c r="P12" s="58">
         <v>1</v>
       </c>
-      <c r="Q12" s="64">
+      <c r="Q12" s="58">
         <v>2</v>
       </c>
-      <c r="R12" s="65">
+      <c r="R12" s="59">
         <v>3</v>
       </c>
     </row>
@@ -2439,19 +2439,19 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="J14" s="45" t="s">
+      <c r="J14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="64"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="50"/>
+      <c r="O14" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1">
       <c r="A15" s="2"/>
@@ -2471,7 +2471,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
       <c r="L16" s="25"/>
-      <c r="M16" s="66">
+      <c r="M16" s="60">
         <f>$F$3*L17</f>
         <v>182.14178609528693</v>
       </c>
@@ -2501,7 +2501,7 @@
         <f>MAX($F$6*($F$5*R16+(1-$F$5)*R18),$C$4-L17)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="61"/>
+      <c r="R17" s="55"/>
     </row>
     <row r="18" spans="1:18">
       <c r="I18" s="14"/>
@@ -2511,7 +2511,7 @@
         <v>122.12461201543867</v>
       </c>
       <c r="L18" s="17"/>
-      <c r="M18" s="55">
+      <c r="M18" s="49">
         <f>$F$4*L17</f>
         <v>128.81474239966511</v>
       </c>
@@ -2530,7 +2530,7 @@
     <row r="19" spans="1:18">
       <c r="A19" s="2"/>
       <c r="J19" s="31">
-        <f>C3</f>
+        <f>$C$3</f>
         <v>100</v>
       </c>
       <c r="K19" s="16"/>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="M19" s="29"/>
       <c r="N19" s="21"/>
-      <c r="O19" s="62">
+      <c r="O19" s="56">
         <f>MAX($F$6*($F$5*P18+(1-$F$5)*P20),$C$4-J19)</f>
         <v>6.6779012271320646</v>
       </c>
@@ -2549,7 +2549,7 @@
         <f>MAX($F$6*($F$5*R18+(1-$F$5)*R20),$C$4-L19)</f>
         <v>2.0623567168718178</v>
       </c>
-      <c r="R19" s="60"/>
+      <c r="R19" s="54"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="2"/>
@@ -2560,7 +2560,7 @@
         <v>86.369255373382117</v>
       </c>
       <c r="L20" s="17"/>
-      <c r="M20" s="55">
+      <c r="M20" s="49">
         <f>$F$4*L19</f>
         <v>91.100665120366031</v>
       </c>
@@ -2593,14 +2593,14 @@
         <f>MAX($F$6*($F$5*R20+(1-$F$5)*R22),$C$4-L21)</f>
         <v>20.403517262475049</v>
       </c>
-      <c r="R21" s="60"/>
+      <c r="R21" s="54"/>
     </row>
     <row r="22" spans="1:18" ht="15" thickBot="1">
       <c r="I22" s="14"/>
       <c r="J22" s="34"/>
       <c r="K22" s="35"/>
       <c r="L22" s="36"/>
-      <c r="M22" s="67">
+      <c r="M22" s="61">
         <f>$F$4*L21</f>
         <v>64.428426675133835</v>
       </c>
@@ -2614,32 +2614,32 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" thickBot="1">
-      <c r="I23" s="51" t="s">
+      <c r="I23" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="58">
-        <v>0</v>
-      </c>
-      <c r="K23" s="63">
+      <c r="J23" s="52">
+        <v>0</v>
+      </c>
+      <c r="K23" s="57">
         <v>1</v>
       </c>
-      <c r="L23" s="64">
+      <c r="L23" s="58">
         <v>2</v>
       </c>
-      <c r="M23" s="65">
+      <c r="M23" s="59">
         <v>3</v>
       </c>
-      <c r="N23" s="52"/>
-      <c r="O23" s="68">
-        <v>0</v>
-      </c>
-      <c r="P23" s="64">
+      <c r="N23" s="46"/>
+      <c r="O23" s="62">
+        <v>0</v>
+      </c>
+      <c r="P23" s="58">
         <v>1</v>
       </c>
-      <c r="Q23" s="64">
+      <c r="Q23" s="58">
         <v>2</v>
       </c>
-      <c r="R23" s="65">
+      <c r="R23" s="59">
         <v>3</v>
       </c>
     </row>

</xml_diff>